<commit_message>
commit Lexus notebook and dataframe after updatings: remove duplicated rows
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_lexus_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_lexus_updated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" t="n">
         <v>2010</v>
@@ -2930,7 +2930,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ISF</t>
+          <t>LX</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -2941,7 +2941,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" t="n">
         <v>2010</v>
@@ -2953,18 +2953,18 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>LX</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Smart Key</t>
+          <t>Std</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" t="n">
         <v>2010</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>GX</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -2987,7 +2987,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" t="n">
         <v>2010</v>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>GX</t>
+          <t>RX</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3010,7 +3010,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" t="n">
         <v>2010</v>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>RX</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3033,10 +3033,10 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3045,18 +3045,18 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Smart Key</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" t="n">
         <v>2011</v>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>GX</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3079,7 +3079,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" t="n">
         <v>2011</v>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>GX</t>
+          <t>LS</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3102,7 +3102,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" t="n">
         <v>2011</v>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>LS</t>
+          <t>RX</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3125,7 +3125,7 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" t="n">
         <v>2011</v>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>RX</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -3148,7 +3148,7 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" t="n">
         <v>2011</v>
@@ -3160,7 +3160,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3171,7 +3171,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" t="n">
         <v>2011</v>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>ISF</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -3194,7 +3194,7 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B121" t="n">
         <v>2011</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>ISF</t>
+          <t>LX</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3217,7 +3217,7 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B122" t="n">
         <v>2011</v>
@@ -3229,21 +3229,21 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>ISF</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Smart Key</t>
+          <t>Std</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B123" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>LX</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3263,10 +3263,10 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B124" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3275,18 +3275,18 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>GX</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Smart Key</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B125" t="n">
         <v>2012</v>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>LS</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3309,7 +3309,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B126" t="n">
         <v>2012</v>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>GX</t>
+          <t>RX</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3332,7 +3332,7 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B127" t="n">
         <v>2012</v>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>LS</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -3355,7 +3355,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B128" t="n">
         <v>2012</v>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>RX</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -3378,7 +3378,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B129" t="n">
         <v>2012</v>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>ISF</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -3401,7 +3401,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B130" t="n">
         <v>2012</v>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>LX</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -3424,7 +3424,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B131" t="n">
         <v>2012</v>
@@ -3436,18 +3436,18 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>ISF</t>
+          <t>LFA</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Smart Key</t>
+          <t>Std</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B132" t="n">
         <v>2012</v>
@@ -3459,21 +3459,21 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>ISF</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Smart Key</t>
+          <t>Std</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B133" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>LX</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -3493,10 +3493,10 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B134" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -3505,21 +3505,21 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>LFA</t>
+          <t>GX</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Smart Key</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B135" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -3528,18 +3528,18 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>LS</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Smart Key</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B136" t="n">
         <v>2013</v>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>RX</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -3562,7 +3562,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B137" t="n">
         <v>2013</v>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>GX</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -3585,7 +3585,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B138" t="n">
         <v>2013</v>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>LS</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -3608,7 +3608,7 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B139" t="n">
         <v>2013</v>
@@ -3620,7 +3620,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>RX</t>
+          <t>ISF</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -3631,7 +3631,7 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B140" t="n">
         <v>2013</v>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>LX</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -3654,7 +3654,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B141" t="n">
         <v>2013</v>
@@ -3666,102 +3666,10 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>LFA</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
-        <is>
-          <t>Smart Key</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B142" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Lexus</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>ISF</t>
-        </is>
-      </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>Smart Key</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B143" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Lexus</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>ISF</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>Smart Key</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>142</v>
-      </c>
-      <c r="B144" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Lexus</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>LX</t>
-        </is>
-      </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>Smart Key</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>143</v>
-      </c>
-      <c r="B145" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Lexus</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>LFA</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr">
         <is>
           <t>Std</t>
         </is>

</xml_diff>